<commit_message>
Added: Download to Excel - pages/index.html
</commit_message>
<xml_diff>
--- a/assets/excelTemplate/datos.xlsx
+++ b/assets/excelTemplate/datos.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$2:$G$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$2:$I$2</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,42 +22,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>unidad</t>
-  </si>
-  <si>
-    <t>placa</t>
-  </si>
-  <si>
-    <t>nombre</t>
-  </si>
-  <si>
-    <t>cedula</t>
-  </si>
-  <si>
-    <t>whatsapp</t>
-  </si>
-  <si>
-    <t>estado</t>
-  </si>
-  <si>
-    <t>role</t>
-  </si>
-  <si>
-    <t>Base de Datos de Personal</t>
-  </si>
-  <si>
-    <t>Fecha:</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Teki Susu - de 12 de Agosto de 2024</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Semana</t>
+  </si>
+  <si>
+    <t>Lunes</t>
+  </si>
+  <si>
+    <t>Martes</t>
+  </si>
+  <si>
+    <t>Miercoles</t>
+  </si>
+  <si>
+    <t>Jueves</t>
+  </si>
+  <si>
+    <t>Viernes</t>
+  </si>
+  <si>
+    <t>Sábado</t>
+  </si>
+  <si>
+    <t>Estado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="[$-580A]dddd\,\ dd&quot; de &quot;mmmm&quot; de &quot;yyyy;@"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -124,15 +124,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -418,39 +415,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="14.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16" style="1" customWidth="1"/>
     <col min="4" max="7" width="14.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="F1" s="1" t="s">
-        <v>8</v>
-      </c>
+    <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
       <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>3</v>
@@ -464,11 +465,17 @@
       <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="H2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:G2"/>
+  <autoFilter ref="A2:I2"/>
   <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>